<commit_message>
fix date for disease recording date
</commit_message>
<xml_diff>
--- a/output/diseaase_record.xlsx
+++ b/output/diseaase_record.xlsx
@@ -107,7 +107,7 @@
     <t/>
   </si>
   <si>
-    <t>43216</t>
+    <t>2018-04-28</t>
   </si>
   <si>
     <t>8.06.2015 - 19.06.2015</t>
@@ -128,34 +128,34 @@
     <t>06.-08.06.2017</t>
   </si>
   <si>
-    <t>43263</t>
+    <t>2018-06-14</t>
   </si>
   <si>
     <t>none</t>
   </si>
   <si>
-    <t>43636</t>
+    <t>2019-06-22</t>
   </si>
   <si>
-    <t>42102</t>
+    <t>2015-04-10</t>
   </si>
   <si>
-    <t>42145</t>
+    <t>2015-05-23</t>
   </si>
   <si>
     <t>BBCH65</t>
   </si>
   <si>
-    <t>42472</t>
+    <t>2016-04-14</t>
   </si>
   <si>
-    <t>42509</t>
+    <t>2016-05-21</t>
   </si>
   <si>
-    <t>42837</t>
+    <t>2017-04-14</t>
   </si>
   <si>
-    <t>42877</t>
+    <t>2017-05-24</t>
   </si>
 </sst>
 </file>

</xml_diff>